<commit_message>
parfor + loadingBar finished + testing
</commit_message>
<xml_diff>
--- a/someexcelfile.xlsx
+++ b/someexcelfile.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="105">
   <si>
     <t>File_Name</t>
   </si>
@@ -74,6 +74,273 @@
   </si>
   <si>
     <t>Number_Of_Cells</t>
+  </si>
+  <si>
+    <t>12.7_09 Cl Fos 4x.tif</t>
+  </si>
+  <si>
+    <t>12.11b_12 Cg1 Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.13b_12 lCPu Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.18a_12 Cl Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.1_19 MPO Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.1_19 MnPO Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.11b_19 MnPO Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.18a_19 Cl Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.18b_19 AI Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.2a_19 Cg2 Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.2b_19 LSV Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.4a_19 Cl Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.7_18 LSV Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.7_18 MPA Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.8_18 AI Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.9b_19 Cg1 Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.9b_19 Cg2 Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.1b_32 Rt Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.11b_32 RSA Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.11a_32 Rt Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.12a_32 DG Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.2_33 LGP.2 Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.2_33 DH-CA2 Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.2a_32 Ect Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.2b_32 RSGb Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.4b_32 CM Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.4a_32 CA1a Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.4a_32 LHb Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.4a_32 PRh Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.7_33 DH-CA1 Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.7a_33 RSGa Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.8_33 DH-CA2 Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.1b_42 DMPAG Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.11b_42 S Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.18a_42 S Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.4a_42 dDGb Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.7b_42 vCA3 Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.8b_42 dDGa Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>12.9b_42 dCA1 Fos 20x.tif</t>
+  </si>
+  <si>
+    <t>09.04.17</t>
+  </si>
+  <si>
+    <t>28.11.17</t>
+  </si>
+  <si>
+    <t>31.10.17</t>
+  </si>
+  <si>
+    <t>09.21.17</t>
+  </si>
+  <si>
+    <t>10.12.17</t>
+  </si>
+  <si>
+    <t>4.12.17</t>
+  </si>
+  <si>
+    <t>4.11.17</t>
+  </si>
+  <si>
+    <t>11.12.17</t>
+  </si>
+  <si>
+    <t>1.11.17</t>
+  </si>
+  <si>
+    <t>27.12.17</t>
+  </si>
+  <si>
+    <t>5.12.17</t>
+  </si>
+  <si>
+    <t>9.11.17</t>
+  </si>
+  <si>
+    <t>10.11.17</t>
+  </si>
+  <si>
+    <t>09.01.17</t>
+  </si>
+  <si>
+    <t>09.03.17</t>
+  </si>
+  <si>
+    <t>12.12.17</t>
+  </si>
+  <si>
+    <t>7.11.17</t>
+  </si>
+  <si>
+    <t>28.12.17</t>
+  </si>
+  <si>
+    <t>7.12.17</t>
+  </si>
+  <si>
+    <t>16.11.17</t>
+  </si>
+  <si>
+    <t>29.12.17</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Cl</t>
+  </si>
+  <si>
+    <t>lCPu</t>
+  </si>
+  <si>
+    <t>MPO</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Cg2</t>
+  </si>
+  <si>
+    <t>LSV</t>
+  </si>
+  <si>
+    <t>MPA</t>
+  </si>
+  <si>
+    <t>Rt</t>
+  </si>
+  <si>
+    <t>RSA</t>
+  </si>
+  <si>
+    <t>DG</t>
+  </si>
+  <si>
+    <t>LGP.2</t>
+  </si>
+  <si>
+    <t>DH-CA2</t>
+  </si>
+  <si>
+    <t>Ect</t>
+  </si>
+  <si>
+    <t>RSGb</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>CA1a</t>
+  </si>
+  <si>
+    <t>LHb</t>
+  </si>
+  <si>
+    <t>PRh</t>
+  </si>
+  <si>
+    <t>DH-CA1</t>
+  </si>
+  <si>
+    <t>RSGa</t>
+  </si>
+  <si>
+    <t>DMPAG</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>dDGb</t>
+  </si>
+  <si>
+    <t>vCA3</t>
+  </si>
+  <si>
+    <t>dDGa</t>
+  </si>
+  <si>
+    <t>dCA1</t>
+  </si>
+  <si>
+    <t>12.13b_12 lCPu DAPI 20x.tif</t>
+  </si>
+  <si>
+    <t>DAPI</t>
   </si>
 </sst>
 </file>
@@ -392,17 +659,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
     <col min="6" max="6" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
@@ -436,48 +703,48 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="B2">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="G2">
         <v>20</v>
       </c>
       <c r="H2">
-        <v>6</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B3">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="G3">
         <v>20</v>
@@ -488,28 +755,1094 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10">
+        <v>20</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>20</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B13">
         <v>19</v>
       </c>
-      <c r="C4">
+      <c r="C13">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
         <v>13</v>
       </c>
-      <c r="G4">
-        <v>20</v>
-      </c>
-      <c r="H4">
+      <c r="G13">
+        <v>20</v>
+      </c>
+      <c r="H13">
         <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14">
+        <v>20</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15">
+        <v>20</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16">
+        <v>20</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17">
+        <v>20</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18">
+        <v>20</v>
+      </c>
+      <c r="H18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19">
+        <v>20</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20">
+        <v>20</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22">
+        <v>20</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23">
+        <v>20</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24">
+        <v>20</v>
+      </c>
+      <c r="H24">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>33</v>
+      </c>
+      <c r="C25">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25">
+        <v>20</v>
+      </c>
+      <c r="H25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>33</v>
+      </c>
+      <c r="C26">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26">
+        <v>20</v>
+      </c>
+      <c r="H26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>33</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27">
+        <v>20</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28">
+        <v>33</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28">
+        <v>20</v>
+      </c>
+      <c r="H28">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29">
+        <v>33</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29">
+        <v>20</v>
+      </c>
+      <c r="H29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <v>33</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30">
+        <v>20</v>
+      </c>
+      <c r="H30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>90</v>
+      </c>
+      <c r="G31">
+        <v>20</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>33</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>91</v>
+      </c>
+      <c r="G32">
+        <v>20</v>
+      </c>
+      <c r="H32">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <v>33</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>92</v>
+      </c>
+      <c r="G33">
+        <v>20</v>
+      </c>
+      <c r="H33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>93</v>
+      </c>
+      <c r="G34">
+        <v>20</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <v>33</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" t="s">
+        <v>94</v>
+      </c>
+      <c r="G35">
+        <v>20</v>
+      </c>
+      <c r="H35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36">
+        <v>33</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" t="s">
+        <v>95</v>
+      </c>
+      <c r="G36">
+        <v>20</v>
+      </c>
+      <c r="H36">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37">
+        <v>33</v>
+      </c>
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" t="s">
+        <v>96</v>
+      </c>
+      <c r="G37">
+        <v>20</v>
+      </c>
+      <c r="H37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38">
+        <v>33</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>88</v>
+      </c>
+      <c r="G38">
+        <v>20</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <v>42</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>97</v>
+      </c>
+      <c r="G39">
+        <v>20</v>
+      </c>
+      <c r="H39">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40">
+        <v>42</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" t="s">
+        <v>98</v>
+      </c>
+      <c r="G40">
+        <v>20</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41">
+        <v>42</v>
+      </c>
+      <c r="C41">
+        <v>18</v>
+      </c>
+      <c r="D41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" t="s">
+        <v>98</v>
+      </c>
+      <c r="G41">
+        <v>20</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42">
+        <v>42</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" t="s">
+        <v>99</v>
+      </c>
+      <c r="G42">
+        <v>20</v>
+      </c>
+      <c r="H42">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" t="s">
+        <v>100</v>
+      </c>
+      <c r="G43">
+        <v>20</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44">
+        <v>42</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>75</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" t="s">
+        <v>101</v>
+      </c>
+      <c r="G44">
+        <v>20</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45">
+        <v>42</v>
+      </c>
+      <c r="C45">
+        <v>9</v>
+      </c>
+      <c r="D45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" t="s">
+        <v>102</v>
+      </c>
+      <c r="G45">
+        <v>20</v>
+      </c>
+      <c r="H45">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>